<commit_message>
Raghav Bansal Changes 17.11.2019 12.06
</commit_message>
<xml_diff>
--- a/uploads/UploadCertificationData.xlsx
+++ b/uploads/UploadCertificationData.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77B477A1-37B0-4DC0-93A2-5B50BCFF632E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66A0DAC-D45D-462D-BF8F-C5EF1B74CB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DRCKJBhPdGH9ntzMEvM0r0cFNcH9EVbCbTGEpR+EB2OHxe6aR8TWxxWJkqGRILb/fDzNDQ0sfXsfmb9xv6y5mg==" workbookSaltValue="0HUrxK8MrZPZMIPAaKNMhw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Participation" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="8">
   <si>
     <t>Sno</t>
   </si>
@@ -45,7 +45,13 @@
     <t>Raghav Bansal</t>
   </si>
   <si>
-    <t>First</t>
+    <t>Surjeet Kumar</t>
+  </si>
+  <si>
+    <t>Puneet Kapoor</t>
+  </si>
+  <si>
+    <t>Fourth</t>
   </si>
 </sst>
 </file>
@@ -417,9 +423,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,9 +457,15 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>17103032</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
@@ -1986,13 +1998,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>17103027</v>
+        <v>17103033</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -2235,9 +2247,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Raghav Bansal Changes 16.12.2019
</commit_message>
<xml_diff>
--- a/uploads/UploadCertificationData.xlsx
+++ b/uploads/UploadCertificationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66A0DAC-D45D-462D-BF8F-C5EF1B74CB45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45270044-2900-4A40-B2A8-DD49A3A7FA77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DRCKJBhPdGH9ntzMEvM0r0cFNcH9EVbCbTGEpR+EB2OHxe6aR8TWxxWJkqGRILb/fDzNDQ0sfXsfmb9xv6y5mg==" workbookSaltValue="0HUrxK8MrZPZMIPAaKNMhw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
@@ -45,13 +45,13 @@
     <t>Raghav Bansal</t>
   </si>
   <si>
-    <t>Surjeet Kumar</t>
+    <t>Jatinder Kumar</t>
   </si>
   <si>
     <t>Puneet Kapoor</t>
   </si>
   <si>
-    <t>Fourth</t>
+    <t>First</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>17103032</v>
+        <v>17103063</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>5</v>
@@ -1966,7 +1966,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2249,7 +2249,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="N19" sqref="M18:N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2273,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>17103027</v>
+        <v>17103032</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>